<commit_message>
Fixed typo in EmbarkedUnits.lua
</commit_message>
<xml_diff>
--- a/newunits.xlsx
+++ b/newunits.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Documents\GitHub\Civ5-RED-Modpack\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nutty\Documents\GitHub\Civ5-RED-Modpack\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -491,7 +491,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3740" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3754" uniqueCount="379">
   <si>
     <t>Model</t>
   </si>
@@ -2211,7 +2211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="158">
+  <cellXfs count="159">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2619,11 +2619,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2640,9 +2640,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2652,10 +2649,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4742,8 +4745,8 @@
   <dimension ref="A1:DP135"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AQ16" sqref="AQ16"/>
+      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AX68" sqref="AX68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4791,18 +4794,18 @@
       </c>
       <c r="M1" s="150"/>
       <c r="N1" s="151"/>
-      <c r="O1" s="153" t="s">
+      <c r="O1" s="152" t="s">
         <v>346</v>
       </c>
-      <c r="P1" s="154"/>
-      <c r="Q1" s="154"/>
-      <c r="R1" s="154"/>
-      <c r="S1" s="154"/>
-      <c r="T1" s="154"/>
-      <c r="U1" s="154"/>
-      <c r="V1" s="154"/>
-      <c r="W1" s="155"/>
-      <c r="X1" s="146" t="s">
+      <c r="P1" s="153"/>
+      <c r="Q1" s="153"/>
+      <c r="R1" s="153"/>
+      <c r="S1" s="153"/>
+      <c r="T1" s="153"/>
+      <c r="U1" s="153"/>
+      <c r="V1" s="153"/>
+      <c r="W1" s="154"/>
+      <c r="X1" s="155" t="s">
         <v>157</v>
       </c>
       <c r="Y1" s="147"/>
@@ -4811,18 +4814,18 @@
       <c r="AB1" s="147"/>
       <c r="AC1" s="147"/>
       <c r="AD1" s="148"/>
-      <c r="AE1" s="153" t="s">
+      <c r="AE1" s="152" t="s">
         <v>347</v>
       </c>
-      <c r="AF1" s="154"/>
-      <c r="AG1" s="154"/>
-      <c r="AH1" s="155"/>
+      <c r="AF1" s="153"/>
+      <c r="AG1" s="153"/>
+      <c r="AH1" s="154"/>
       <c r="AI1" s="149" t="s">
         <v>350</v>
       </c>
       <c r="AJ1" s="150"/>
       <c r="AK1" s="151"/>
-      <c r="AL1" s="146" t="s">
+      <c r="AL1" s="155" t="s">
         <v>7</v>
       </c>
       <c r="AM1" s="147"/>
@@ -4833,12 +4836,12 @@
       <c r="AR1" s="147"/>
       <c r="AS1" s="147"/>
       <c r="AT1" s="148"/>
-      <c r="AU1" s="146" t="s">
+      <c r="AU1" s="155" t="s">
         <v>348</v>
       </c>
       <c r="AV1" s="147"/>
       <c r="AW1" s="148"/>
-      <c r="AX1" s="146" t="s">
+      <c r="AX1" s="155" t="s">
         <v>349</v>
       </c>
       <c r="AY1" s="147"/>
@@ -4958,10 +4961,10 @@
       <c r="BC2" s="36" t="s">
         <v>317</v>
       </c>
-      <c r="BD2" s="152" t="s">
+      <c r="BD2" s="157" t="s">
         <v>315</v>
       </c>
-      <c r="BE2" s="152"/>
+      <c r="BE2" s="157"/>
     </row>
     <row r="3" spans="1:114" s="2" customFormat="1" ht="112.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
@@ -5281,10 +5284,10 @@
         <v>343</v>
       </c>
       <c r="BC5" s="23"/>
-      <c r="BD5" s="145" t="s">
+      <c r="BD5" s="156" t="s">
         <v>330</v>
       </c>
-      <c r="BE5" s="145"/>
+      <c r="BE5" s="156"/>
       <c r="BF5" s="10"/>
       <c r="BG5" s="10"/>
       <c r="BH5" s="10"/>
@@ -5812,7 +5815,7 @@
       <c r="D11" s="53"/>
       <c r="E11" s="53"/>
       <c r="F11" s="53"/>
-      <c r="G11" s="53" t="s">
+      <c r="G11" s="67" t="s">
         <v>328</v>
       </c>
       <c r="H11" s="71" t="s">
@@ -6288,7 +6291,7 @@
         <v>238</v>
       </c>
       <c r="B17" s="22"/>
-      <c r="C17" s="156" t="s">
+      <c r="C17" s="145" t="s">
         <v>328</v>
       </c>
       <c r="D17" s="51"/>
@@ -8506,7 +8509,7 @@
         <v>239</v>
       </c>
       <c r="B37" s="22"/>
-      <c r="C37" s="156" t="s">
+      <c r="C37" s="145" t="s">
         <v>328</v>
       </c>
       <c r="D37" s="51"/>
@@ -8889,7 +8892,7 @@
         <v>230</v>
       </c>
       <c r="B40" s="22"/>
-      <c r="C40" s="157"/>
+      <c r="C40" s="146"/>
       <c r="D40" s="91"/>
       <c r="E40" s="53" t="s">
         <v>328</v>
@@ -9014,7 +9017,7 @@
         <v>232</v>
       </c>
       <c r="B41" s="22"/>
-      <c r="C41" s="156" t="s">
+      <c r="C41" s="145" t="s">
         <v>328</v>
       </c>
       <c r="D41" s="51"/>
@@ -9351,7 +9354,7 @@
         <v>234</v>
       </c>
       <c r="B44" s="22"/>
-      <c r="C44" s="156" t="s">
+      <c r="C44" s="145" t="s">
         <v>328</v>
       </c>
       <c r="D44" s="51"/>
@@ -11099,13 +11102,27 @@
       <c r="U63" s="60"/>
       <c r="V63" s="60"/>
       <c r="W63" s="106"/>
-      <c r="X63" s="114"/>
-      <c r="Y63" s="60"/>
-      <c r="Z63" s="60"/>
-      <c r="AA63" s="60"/>
-      <c r="AB63" s="60"/>
-      <c r="AC63" s="60"/>
-      <c r="AD63" s="107"/>
+      <c r="X63" s="110" t="s">
+        <v>356</v>
+      </c>
+      <c r="Y63" s="61" t="s">
+        <v>343</v>
+      </c>
+      <c r="Z63" s="61" t="s">
+        <v>343</v>
+      </c>
+      <c r="AA63" s="61" t="s">
+        <v>343</v>
+      </c>
+      <c r="AB63" s="61" t="s">
+        <v>343</v>
+      </c>
+      <c r="AC63" s="61" t="s">
+        <v>343</v>
+      </c>
+      <c r="AD63" s="107" t="s">
+        <v>343</v>
+      </c>
       <c r="AE63" s="114"/>
       <c r="AF63" s="60"/>
       <c r="AG63" s="60"/>
@@ -11663,13 +11680,27 @@
       <c r="AT68" s="123" t="s">
         <v>343</v>
       </c>
-      <c r="AU68" s="114"/>
-      <c r="AV68" s="60"/>
-      <c r="AW68" s="107"/>
-      <c r="AX68" s="129"/>
-      <c r="AY68" s="60"/>
-      <c r="AZ68" s="60"/>
-      <c r="BA68" s="106"/>
+      <c r="AU68" s="110" t="s">
+        <v>356</v>
+      </c>
+      <c r="AV68" s="61" t="s">
+        <v>343</v>
+      </c>
+      <c r="AW68" s="107" t="s">
+        <v>343</v>
+      </c>
+      <c r="AX68" s="158" t="s">
+        <v>356</v>
+      </c>
+      <c r="AY68" s="61" t="s">
+        <v>343</v>
+      </c>
+      <c r="AZ68" s="61" t="s">
+        <v>343</v>
+      </c>
+      <c r="BA68" s="107" t="s">
+        <v>343</v>
+      </c>
       <c r="BB68" s="106"/>
       <c r="BC68" s="23"/>
       <c r="BD68" s="23"/>
@@ -19161,17 +19192,17 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="11">
-    <mergeCell ref="B1:K1"/>
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="O1:W1"/>
-    <mergeCell ref="X1:AD1"/>
-    <mergeCell ref="AE1:AH1"/>
     <mergeCell ref="BD5:BE5"/>
     <mergeCell ref="AX1:BA1"/>
     <mergeCell ref="AI1:AK1"/>
     <mergeCell ref="AL1:AT1"/>
     <mergeCell ref="AU1:AW1"/>
     <mergeCell ref="BD2:BE2"/>
+    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="O1:W1"/>
+    <mergeCell ref="X1:AD1"/>
+    <mergeCell ref="AE1:AH1"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>